<commit_message>
Create districts and streets repository
</commit_message>
<xml_diff>
--- a/Semestr 4/Języki i paradygmaty programowania/TrafficApp/Koordynaty_Ulic.xlsx
+++ b/Semestr 4/Języki i paradygmaty programowania/TrafficApp/Koordynaty_Ulic.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programowanie\SAN\Semestr 4\Języki i paradygmaty programowania\TrafficApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CECFDA3-9867-43F3-AA0B-F87600F3EA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E6B08-12A1-481E-9322-F946685B1B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9AA3918B-8562-4D28-8A85-572A34A2D5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Koordynaty" sheetId="1" r:id="rId1"/>
     <sheet name="Konwersja_Y" sheetId="3" r:id="rId2"/>
+    <sheet name="Osiedla" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
   <si>
     <t>Przelicznik</t>
   </si>
@@ -103,6 +104,30 @@
   </si>
   <si>
     <t>Coord_gimp</t>
+  </si>
+  <si>
+    <t>Osiedle Dolnośląskie</t>
+  </si>
+  <si>
+    <t>Czapliniec</t>
+  </si>
+  <si>
+    <t>Edwardów</t>
+  </si>
+  <si>
+    <t>Osiedle Kopernika</t>
+  </si>
+  <si>
+    <t>Osiedle Okrzei</t>
+  </si>
+  <si>
+    <t>Osiedle Słoneczne</t>
+  </si>
+  <si>
+    <t>Śródmieście</t>
+  </si>
+  <si>
+    <t>Osiedle</t>
   </si>
 </sst>
 </file>
@@ -284,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -302,6 +327,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -639,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C650E18-CD7E-4D8F-9C77-AFD0E727F83A}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,28 +679,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="H1" s="17" t="s">
+      <c r="F1" s="16"/>
+      <c r="H1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
@@ -687,10 +713,10 @@
       <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -715,10 +741,10 @@
       <c r="F3" s="12">
         <v>37</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="15">
         <v>-28</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="15">
         <v>-27</v>
       </c>
     </row>
@@ -1330,7 +1356,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>14</v>
       </c>
@@ -1352,7 +1378,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>14</v>
       </c>
@@ -1374,7 +1400,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11" t="s">
         <v>18</v>
@@ -1394,7 +1420,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>14</v>
       </c>
@@ -1414,6 +1440,14 @@
       </c>
       <c r="F36" s="11">
         <v>227</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" ref="K4:K36" si="2">B36</f>
+        <v>Wojska Polskiego</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" ref="L4:L36" si="3">"{ "&amp;C36&amp;", "&amp;D36&amp;" }"</f>
+        <v>{ 111, 6 }</v>
       </c>
     </row>
   </sheetData>
@@ -1434,7 +1468,7 @@
   <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,11 +1491,11 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>A3+1</f>
+        <f t="shared" ref="A2:A7" si="0">A3+1</f>
         <v>212</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="A2:B71" si="0">B3-1</f>
+        <f t="shared" ref="B2:B71" si="1">B3-1</f>
         <v>-6</v>
       </c>
       <c r="C2">
@@ -1470,11 +1504,11 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>211</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="C3">
@@ -1483,11 +1517,11 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="C4">
@@ -1496,11 +1530,11 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="C5">
@@ -1509,11 +1543,11 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="C6">
@@ -1522,11 +1556,11 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>207</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="C7">
@@ -1538,7 +1572,7 @@
         <v>206</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C8">
@@ -1551,7 +1585,7 @@
         <v>205</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C9">
@@ -1560,11 +1594,11 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ref="A10:A73" si="1">A9-1</f>
+        <f t="shared" ref="A10:A73" si="2">A9-1</f>
         <v>204</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C10">
@@ -1573,11 +1607,11 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>203</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C11">
@@ -1586,11 +1620,11 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>202</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C12">
@@ -1599,11 +1633,11 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>201</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C13">
@@ -1612,11 +1646,11 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C14">
@@ -1625,11 +1659,11 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>199</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C15">
@@ -1638,11 +1672,11 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C16">
@@ -1651,11 +1685,11 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C17">
@@ -1664,11 +1698,11 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C18">
@@ -1677,11 +1711,11 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C19">
@@ -1690,11 +1724,11 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>194</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C20">
@@ -1703,11 +1737,11 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>193</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C21">
@@ -1716,11 +1750,11 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C22">
@@ -1729,11 +1763,11 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>191</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C23">
@@ -1742,11 +1776,11 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C24">
@@ -1755,11 +1789,11 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>189</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C25">
@@ -1768,11 +1802,11 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C26">
@@ -1781,11 +1815,11 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>187</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C27">
@@ -1794,11 +1828,11 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>186</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C28">
@@ -1807,11 +1841,11 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>185</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C29">
@@ -1820,11 +1854,11 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C30">
@@ -1833,11 +1867,11 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>183</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C31">
@@ -1846,11 +1880,11 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>182</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C32">
@@ -1859,11 +1893,11 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C33">
@@ -1872,11 +1906,11 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C34">
@@ -1885,11 +1919,11 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>179</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C35">
@@ -1898,11 +1932,11 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>178</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C36">
@@ -1911,11 +1945,11 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>177</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C37">
@@ -1924,11 +1958,11 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C38">
@@ -1937,11 +1971,11 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>175</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C39">
@@ -1950,11 +1984,11 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C40">
@@ -1963,11 +1997,11 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C41">
@@ -1976,11 +2010,11 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C42">
@@ -1989,11 +2023,11 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>171</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C43">
@@ -2002,11 +2036,11 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C44">
@@ -2015,11 +2049,11 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C45">
@@ -2028,11 +2062,11 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C46">
@@ -2041,11 +2075,11 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C47">
@@ -2054,11 +2088,11 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C48">
@@ -2067,11 +2101,11 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C49">
@@ -2080,11 +2114,11 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C50">
@@ -2093,11 +2127,11 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>163</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="C51">
@@ -2106,11 +2140,11 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>162</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="C52">
@@ -2119,11 +2153,11 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>161</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C53">
@@ -2132,11 +2166,11 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C54">
@@ -2145,11 +2179,11 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C55">
@@ -2158,11 +2192,11 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>158</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C56">
@@ -2171,11 +2205,11 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C57">
@@ -2184,11 +2218,11 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C58">
@@ -2197,11 +2231,11 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C59">
@@ -2210,11 +2244,11 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>154</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="C60">
@@ -2223,11 +2257,11 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="B61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="C61">
@@ -2236,11 +2270,11 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="B62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C62">
@@ -2249,11 +2283,11 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>151</v>
       </c>
       <c r="B63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C63">
@@ -2262,11 +2296,11 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="B64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C64">
@@ -2275,11 +2309,11 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>149</v>
       </c>
       <c r="B65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="C65">
@@ -2288,11 +2322,11 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="B66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="C66">
@@ -2301,11 +2335,11 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="B67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="C67">
@@ -2314,11 +2348,11 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146</v>
       </c>
       <c r="B68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C68">
@@ -2327,11 +2361,11 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
       <c r="B69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C69">
@@ -2340,11 +2374,11 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="B70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="C70">
@@ -2353,11 +2387,11 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>143</v>
       </c>
       <c r="B71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C71">
@@ -2366,11 +2400,11 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="A72:B135" si="2">B73-1</f>
+        <f t="shared" ref="B72:B135" si="3">B73-1</f>
         <v>64</v>
       </c>
       <c r="C72">
@@ -2379,11 +2413,11 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>141</v>
       </c>
       <c r="B73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="C73">
@@ -2392,11 +2426,11 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" ref="A74:A137" si="3">A73-1</f>
+        <f t="shared" ref="A74:A137" si="4">A73-1</f>
         <v>140</v>
       </c>
       <c r="B74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="C74">
@@ -2405,11 +2439,11 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="B75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="C75">
@@ -2418,11 +2452,11 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138</v>
       </c>
       <c r="B76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="C76">
@@ -2431,11 +2465,11 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
       <c r="B77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="C77">
@@ -2444,11 +2478,11 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
       <c r="B78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="C78">
@@ -2457,11 +2491,11 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>135</v>
       </c>
       <c r="B79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C79">
@@ -2470,11 +2504,11 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>134</v>
       </c>
       <c r="B80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="C80">
@@ -2483,11 +2517,11 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
       <c r="B81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="C81">
@@ -2496,11 +2530,11 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
       <c r="B82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="C82">
@@ -2509,11 +2543,11 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131</v>
       </c>
       <c r="B83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="C83">
@@ -2522,11 +2556,11 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="B84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="C84">
@@ -2535,11 +2569,11 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="B85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="C85">
@@ -2548,11 +2582,11 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="C86">
@@ -2561,11 +2595,11 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="B87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="C87">
@@ -2574,11 +2608,11 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="B88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C88">
@@ -2587,11 +2621,11 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="B89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="C89">
@@ -2600,11 +2634,11 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124</v>
       </c>
       <c r="B90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="C90">
@@ -2613,11 +2647,11 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>123</v>
       </c>
       <c r="B91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="C91">
@@ -2626,11 +2660,11 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122</v>
       </c>
       <c r="B92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="C92">
@@ -2639,11 +2673,11 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>121</v>
       </c>
       <c r="B93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="C93">
@@ -2652,11 +2686,11 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="B94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="C94">
@@ -2665,11 +2699,11 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="B95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="C95">
@@ -2678,11 +2712,11 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>118</v>
       </c>
       <c r="B96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="C96">
@@ -2691,11 +2725,11 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="B97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
       <c r="C97">
@@ -2704,11 +2738,11 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>116</v>
       </c>
       <c r="B98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="C98">
@@ -2717,11 +2751,11 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115</v>
       </c>
       <c r="B99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="C99">
@@ -2730,11 +2764,11 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
       <c r="B100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="C100">
@@ -2743,11 +2777,11 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>113</v>
       </c>
       <c r="B101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="C101">
@@ -2756,11 +2790,11 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="B102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="C102">
@@ -2769,11 +2803,11 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>111</v>
       </c>
       <c r="B103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="C103">
@@ -2782,11 +2816,11 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="B104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="C104">
@@ -2795,11 +2829,11 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
       <c r="B105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="C105">
@@ -2808,11 +2842,11 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="B106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="C106">
@@ -2821,11 +2855,11 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
       <c r="B107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="C107">
@@ -2834,11 +2868,11 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="B108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="C108">
@@ -2847,11 +2881,11 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="B109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="C109">
@@ -2860,11 +2894,11 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
       <c r="B110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="C110">
@@ -2873,11 +2907,11 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
       <c r="B111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="C111">
@@ -2886,11 +2920,11 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="B112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="C112">
@@ -2899,11 +2933,11 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="B113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="C113">
@@ -2912,11 +2946,11 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="B114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="C114">
@@ -2925,11 +2959,11 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="B115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="C115">
@@ -2938,11 +2972,11 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="B116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="C116">
@@ -2951,11 +2985,11 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="B117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="C117">
@@ -2964,11 +2998,11 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="B118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="C118">
@@ -2977,11 +3011,11 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="B119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="C119">
@@ -2990,11 +3024,11 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="B120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="C120">
@@ -3003,11 +3037,11 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="B121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="C121">
@@ -3016,11 +3050,11 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
       <c r="B122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="C122">
@@ -3029,11 +3063,11 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="B123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="C123">
@@ -3042,11 +3076,11 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="B124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="C124">
@@ -3055,11 +3089,11 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="B125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="C125">
@@ -3068,11 +3102,11 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="B126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="C126">
@@ -3081,11 +3115,11 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="B127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="C127">
@@ -3094,11 +3128,11 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
       <c r="B128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="C128">
@@ -3107,11 +3141,11 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="B129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="C129">
@@ -3120,11 +3154,11 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="B130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="C130">
@@ -3133,11 +3167,11 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="B131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="C131">
@@ -3146,11 +3180,11 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="B132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="C132">
@@ -3159,11 +3193,11 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="B133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="C133">
@@ -3172,11 +3206,11 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="C134">
@@ -3185,11 +3219,11 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="C135">
@@ -3198,11 +3232,11 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B136">
-        <f t="shared" ref="A136:B199" si="4">B137-1</f>
+        <f t="shared" ref="B136:B199" si="5">B137-1</f>
         <v>128</v>
       </c>
       <c r="C136">
@@ -3211,11 +3245,11 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="B137">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>129</v>
       </c>
       <c r="C137">
@@ -3224,11 +3258,11 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
-        <f t="shared" ref="A138:A201" si="5">A137-1</f>
+        <f t="shared" ref="A138:A201" si="6">A137-1</f>
         <v>76</v>
       </c>
       <c r="B138">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
       <c r="C138">
@@ -3237,11 +3271,11 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="B139">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>131</v>
       </c>
       <c r="C139">
@@ -3250,11 +3284,11 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="B140">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>132</v>
       </c>
       <c r="C140">
@@ -3263,11 +3297,11 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="B141">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
       <c r="C141">
@@ -3276,11 +3310,11 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="B142">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="C142">
@@ -3289,11 +3323,11 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="B143">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>135</v>
       </c>
       <c r="C143">
@@ -3302,11 +3336,11 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="B144">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>136</v>
       </c>
       <c r="C144">
@@ -3315,11 +3349,11 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="B145">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
       <c r="C145">
@@ -3328,11 +3362,11 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="B146">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>138</v>
       </c>
       <c r="C146">
@@ -3341,11 +3375,11 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="B147">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>139</v>
       </c>
       <c r="C147">
@@ -3354,11 +3388,11 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="B148">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="C148">
@@ -3367,11 +3401,11 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="B149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141</v>
       </c>
       <c r="C149">
@@ -3380,11 +3414,11 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="B150">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>142</v>
       </c>
       <c r="C150">
@@ -3393,11 +3427,11 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="B151">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="C151">
@@ -3406,11 +3440,11 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="B152">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="C152">
@@ -3419,11 +3453,11 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="B153">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="C153">
@@ -3432,11 +3466,11 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="B154">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="C154">
@@ -3445,11 +3479,11 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="B155">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="C155">
@@ -3458,11 +3492,11 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="B156">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="C156">
@@ -3471,11 +3505,11 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="B157">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>149</v>
       </c>
       <c r="C157">
@@ -3484,11 +3518,11 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="B158">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="C158">
@@ -3497,11 +3531,11 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="B159">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>151</v>
       </c>
       <c r="C159">
@@ -3510,11 +3544,11 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="B160">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>152</v>
       </c>
       <c r="C160">
@@ -3523,11 +3557,11 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="B161">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="C161">
@@ -3536,11 +3570,11 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52</v>
       </c>
       <c r="B162">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="C162">
@@ -3549,11 +3583,11 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
       <c r="B163">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
       <c r="C163">
@@ -3562,11 +3596,11 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="B164">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
       <c r="C164">
@@ -3575,11 +3609,11 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
       <c r="B165">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="C165">
@@ -3588,11 +3622,11 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="B166">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>158</v>
       </c>
       <c r="C166">
@@ -3601,11 +3635,11 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="B167">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="C167">
@@ -3614,11 +3648,11 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="B168">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="C168">
@@ -3627,11 +3661,11 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="B169">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="C169">
@@ -3640,11 +3674,11 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="B170">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="C170">
@@ -3653,11 +3687,11 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="B171">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="C171">
@@ -3666,11 +3700,11 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="B172">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="C172">
@@ -3679,11 +3713,11 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="B173">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="C173">
@@ -3692,11 +3726,11 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="B174">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="C174">
@@ -3705,11 +3739,11 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="B175">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="C175">
@@ -3718,11 +3752,11 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="B176">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="C176">
@@ -3731,11 +3765,11 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="B177">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="C177">
@@ -3744,11 +3778,11 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="B178">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="C178">
@@ -3757,11 +3791,11 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="B179">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="C179">
@@ -3770,11 +3804,11 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="B180">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="C180">
@@ -3783,11 +3817,11 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="B181">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
       <c r="C181">
@@ -3796,11 +3830,11 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="B182">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="C182">
@@ -3809,11 +3843,11 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="B183">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="C183">
@@ -3822,11 +3856,11 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="B184">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="C184">
@@ -3835,11 +3869,11 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="B185">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="C185">
@@ -3848,11 +3882,11 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="B186">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="C186">
@@ -3861,11 +3895,11 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="B187">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
       <c r="C187">
@@ -3874,11 +3908,11 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="B188">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="C188">
@@ -3887,11 +3921,11 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="B189">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="C189">
@@ -3900,11 +3934,11 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="B190">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="C190">
@@ -3913,11 +3947,11 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="B191">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="C191">
@@ -3926,11 +3960,11 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="B192">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="C192">
@@ -3939,11 +3973,11 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="B193">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="C193">
@@ -3952,11 +3986,11 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="B194">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="C194">
@@ -3965,11 +3999,11 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="B195">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="C195">
@@ -3978,11 +4012,11 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="B196">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="C196">
@@ -3991,11 +4025,11 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="B197">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="C197">
@@ -4004,11 +4038,11 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="B198">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="C198">
@@ -4017,11 +4051,11 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="B199">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="C199">
@@ -4030,11 +4064,11 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="B200">
-        <f t="shared" ref="A200:B212" si="6">B201-1</f>
+        <f t="shared" ref="B200:B212" si="7">B201-1</f>
         <v>192</v>
       </c>
       <c r="C200">
@@ -4043,11 +4077,11 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="B201">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>193</v>
       </c>
       <c r="C201">
@@ -4056,11 +4090,11 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
-        <f t="shared" ref="A202:A214" si="7">A201-1</f>
+        <f t="shared" ref="A202:A214" si="8">A201-1</f>
         <v>12</v>
       </c>
       <c r="B202">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="C202">
@@ -4069,11 +4103,11 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="B203">
         <f t="shared" si="7"/>
-        <v>11</v>
-      </c>
-      <c r="B203">
-        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="C203">
@@ -4082,11 +4116,11 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="B204">
         <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="B204">
-        <f t="shared" si="6"/>
         <v>196</v>
       </c>
       <c r="C204">
@@ -4095,11 +4129,11 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="B205">
         <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="B205">
-        <f t="shared" si="6"/>
         <v>197</v>
       </c>
       <c r="C205">
@@ -4108,11 +4142,11 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="B206">
         <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="B206">
-        <f t="shared" si="6"/>
         <v>198</v>
       </c>
       <c r="C206">
@@ -4121,11 +4155,11 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="B207">
         <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="B207">
-        <f t="shared" si="6"/>
         <v>199</v>
       </c>
       <c r="C207">
@@ -4134,11 +4168,11 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="B208">
         <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="B208">
-        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="C208">
@@ -4147,11 +4181,11 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="B209">
         <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="B209">
-        <f t="shared" si="6"/>
         <v>201</v>
       </c>
       <c r="C209">
@@ -4160,11 +4194,11 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B210">
         <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B210">
-        <f t="shared" si="6"/>
         <v>202</v>
       </c>
       <c r="C210">
@@ -4173,11 +4207,11 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="B211">
         <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="B211">
-        <f t="shared" si="6"/>
         <v>203</v>
       </c>
       <c r="C211">
@@ -4186,11 +4220,11 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="B212">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="B212">
-        <f t="shared" si="6"/>
         <v>204</v>
       </c>
       <c r="C212">
@@ -4199,7 +4233,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="B213">
@@ -4212,7 +4246,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="B214">
@@ -4225,4 +4259,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00E7580-7FA1-42FD-8F16-F3FEB8BEF1A2}">
+  <dimension ref="B1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>